<commit_message>
clean config, update readme
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -54,9 +54,6 @@
     <t>copy</t>
   </si>
   <si>
-    <t>-preset slow -crf 23</t>
-  </si>
-  <si>
     <t>destination_file</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>destination_folder</t>
   </si>
   <si>
-    <t>Mickeys_clubhuis.S01E01.Katrien_telt_schaapjes</t>
-  </si>
-  <si>
     <t>C:\Program Files\ffmpeg\bin\ffmpeg.exe</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>d:\</t>
+  </si>
+  <si>
+    <t>-preset slow -crf 23 -vf scale=-1:720</t>
+  </si>
+  <si>
+    <t>output_filename</t>
   </si>
 </sst>
 </file>
@@ -464,18 +464,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,17 +504,15 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="27.140625" style="1" customWidth="1"/>
@@ -534,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -549,40 +547,40 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -591,7 +589,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -603,7 +601,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -615,7 +613,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -627,7 +625,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -639,7 +637,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -651,7 +649,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -663,7 +661,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -675,7 +673,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -687,7 +685,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -699,7 +697,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -711,7 +709,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -723,7 +721,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -735,7 +733,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -747,7 +745,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -759,7 +757,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -771,7 +769,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -783,7 +781,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -795,7 +793,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -807,7 +805,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -819,7 +817,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -831,7 +829,7 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -843,7 +841,7 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -855,7 +853,7 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -867,7 +865,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -879,7 +877,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -891,7 +889,7 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -903,7 +901,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>

</xml_diff>